<commit_message>
fields: Define fields in Django app setting, use to show in web UI
Show when viewing or moderating record
</commit_message>
<xml_diff>
--- a/jsondataferretexampleapp/spreadsheetform_guides/project.xlsx
+++ b/jsondataferretexampleapp/spreadsheetform_guides/project.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Outcomes" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t xml:space="preserve">Record Status</t>
   </si>
@@ -86,6 +87,18 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:launch_date/status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome Definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcomes:outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcomes:definition</t>
   </si>
 </sst>
 </file>
@@ -128,6 +141,7 @@
       <color rgb="FF4C4C4C"/>
       <name val="Ubuntu"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -280,12 +294,12 @@
   <dimension ref="A2:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.93"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
@@ -469,4 +483,185 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:B38"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>